<commit_message>
Validacion de la solicitud
</commit_message>
<xml_diff>
--- a/Data/PrebasShell.xlsx
+++ b/Data/PrebasShell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Nombre</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>lujan basilio jose guillermo</t>
+  </si>
+  <si>
+    <t>11/07/1994</t>
+  </si>
+  <si>
+    <t>iztacalco</t>
   </si>
 </sst>
 </file>
@@ -144,11 +150,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -432,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +447,7 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.7109375" customWidth="1"/>
@@ -506,8 +512,8 @@
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3">
-        <v>34526</v>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -525,7 +531,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>15</v>
@@ -646,7 +652,6 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>

</xml_diff>